<commit_message>
peq alteracoes e melhorias
</commit_message>
<xml_diff>
--- a/sources/excel/calculo.xlsx
+++ b/sources/excel/calculo.xlsx
@@ -30,7 +30,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,6 +41,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -72,12 +78,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -385,17 +394,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="4.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="4.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2">
         <v>7073</v>
       </c>
@@ -411,7 +420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -419,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2">
         <v>39798</v>
       </c>
@@ -427,7 +436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2">
         <v>42109</v>
       </c>
@@ -435,7 +444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2">
         <v>53511</v>
       </c>
@@ -443,7 +452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2">
         <v>59057</v>
       </c>
@@ -451,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2">
         <v>59645</v>
       </c>
@@ -459,7 +468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2">
         <v>60831</v>
       </c>
@@ -467,11 +476,27 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="2">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="3">
+        <v>34343</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="3">
+        <v>3222</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="2">
         <v>60985</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B12" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>